<commit_message>
Added multiple coach support
</commit_message>
<xml_diff>
--- a/EvalTemplate.xlsx
+++ b/EvalTemplate.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF69ADB-5B01-4FCE-A255-719E36BD3A42}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71375BCB-BEA8-4D70-B41C-70A68AB3488D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
   <si>
     <t>PlayerName</t>
   </si>
@@ -136,9 +136,6 @@
     <t>End of Fall 2018</t>
   </si>
   <si>
-    <t>Coach</t>
-  </si>
-  <si>
     <t>End of Fall 2019</t>
   </si>
   <si>
@@ -161,6 +158,18 @@
   </si>
   <si>
     <t>Always plays with a smile</t>
+  </si>
+  <si>
+    <t>Coach1</t>
+  </si>
+  <si>
+    <t>Coach2</t>
+  </si>
+  <si>
+    <t>I think he dislikes hotdogs</t>
+  </si>
+  <si>
+    <t>Giggles when he dribbles</t>
   </si>
 </sst>
 </file>
@@ -478,12 +487,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AK4"/>
+  <dimension ref="A1:AK6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
-      <pane xSplit="1350" topLeftCell="U1" activePane="topRight"/>
-      <selection activeCell="AK9" sqref="AK9"/>
-      <selection pane="topRight" activeCell="AK3" sqref="AK3"/>
+      <pane xSplit="1350" activePane="topRight"/>
+      <selection activeCell="AK5" sqref="A5:XFD6"/>
+      <selection pane="topRight" activeCell="AJ6" sqref="AJ6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,7 +615,7 @@
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2">
         <v>2003</v>
@@ -615,7 +624,7 @@
         <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E2">
         <v>5</v>
@@ -714,21 +723,21 @@
         <v>2</v>
       </c>
       <c r="AK2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3">
         <v>2004</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -827,51 +836,277 @@
         <v>3</v>
       </c>
       <c r="AK3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4">
         <v>2003</v>
       </c>
       <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
         <v>40</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>5</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <v>3</v>
+      </c>
+      <c r="M4">
+        <v>4</v>
+      </c>
+      <c r="AK4" t="s">
         <v>41</v>
       </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-      <c r="F4">
-        <v>5</v>
-      </c>
-      <c r="G4">
-        <v>5</v>
-      </c>
-      <c r="H4">
-        <v>5</v>
-      </c>
-      <c r="I4">
-        <v>5</v>
-      </c>
-      <c r="J4">
-        <v>5</v>
-      </c>
-      <c r="K4">
-        <v>3</v>
-      </c>
-      <c r="L4">
-        <v>3</v>
-      </c>
-      <c r="M4">
-        <v>4</v>
-      </c>
-      <c r="AK4" t="s">
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>42</v>
+      </c>
+      <c r="B5">
+        <v>2003</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <v>4</v>
+      </c>
+      <c r="L5">
+        <v>5</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <v>3</v>
+      </c>
+      <c r="O5">
+        <v>4</v>
+      </c>
+      <c r="P5">
+        <v>5</v>
+      </c>
+      <c r="Q5">
+        <v>2</v>
+      </c>
+      <c r="R5">
+        <v>2</v>
+      </c>
+      <c r="S5">
+        <v>3</v>
+      </c>
+      <c r="T5">
+        <v>3</v>
+      </c>
+      <c r="U5">
+        <v>4</v>
+      </c>
+      <c r="V5">
+        <v>4</v>
+      </c>
+      <c r="W5">
+        <v>5</v>
+      </c>
+      <c r="X5">
+        <v>5</v>
+      </c>
+      <c r="Y5">
+        <v>4</v>
+      </c>
+      <c r="Z5">
+        <v>4</v>
+      </c>
+      <c r="AA5">
+        <v>3</v>
+      </c>
+      <c r="AB5">
+        <v>3</v>
+      </c>
+      <c r="AC5">
+        <v>2</v>
+      </c>
+      <c r="AD5">
+        <v>2</v>
+      </c>
+      <c r="AE5">
+        <v>1</v>
+      </c>
+      <c r="AF5">
+        <v>1</v>
+      </c>
+      <c r="AG5">
+        <v>2</v>
+      </c>
+      <c r="AH5">
+        <v>3</v>
+      </c>
+      <c r="AI5">
+        <v>4</v>
+      </c>
+      <c r="AJ5">
+        <v>5</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6">
+        <v>2004</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="M6">
+        <v>3</v>
+      </c>
+      <c r="N6">
+        <v>5</v>
+      </c>
+      <c r="O6">
+        <v>4</v>
+      </c>
+      <c r="P6">
+        <v>4</v>
+      </c>
+      <c r="Q6">
+        <v>3</v>
+      </c>
+      <c r="R6">
+        <v>2</v>
+      </c>
+      <c r="S6">
+        <v>3</v>
+      </c>
+      <c r="T6">
+        <v>4</v>
+      </c>
+      <c r="U6">
+        <v>2</v>
+      </c>
+      <c r="V6">
+        <v>3</v>
+      </c>
+      <c r="W6">
+        <v>4</v>
+      </c>
+      <c r="X6">
+        <v>2</v>
+      </c>
+      <c r="Y6">
+        <v>1</v>
+      </c>
+      <c r="Z6">
+        <v>3</v>
+      </c>
+      <c r="AA6">
+        <v>2</v>
+      </c>
+      <c r="AB6">
+        <v>4</v>
+      </c>
+      <c r="AC6">
+        <v>3</v>
+      </c>
+      <c r="AD6">
+        <v>5</v>
+      </c>
+      <c r="AE6">
+        <v>5</v>
+      </c>
+      <c r="AF6">
+        <v>3</v>
+      </c>
+      <c r="AG6">
+        <v>2</v>
+      </c>
+      <c r="AH6">
+        <v>1</v>
+      </c>
+      <c r="AI6">
+        <v>3</v>
+      </c>
+      <c r="AJ6">
+        <v>3</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>